<commit_message>
feat: migrate PO query system to PostgreSQL and add substations data files
</commit_message>
<xml_diff>
--- a/06.adhoc.requests/18.substations/Subcontractor_Details_substations_equipment.xlsx
+++ b/06.adhoc.requests/18.substations/Subcontractor_Details_substations_equipment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rowadmodern-my.sharepoint.com/personal/omar_essam_rowad-rme_com/Documents/x004 Data Science/03.rme.db/00.repo/rme.db/06.adhoc.requests/18.substations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1257172F-23D5-4CA5-87EE-B0EF93EC9159}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7174F25-C307-442D-9DE0-8D418B4A020A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,6 +332,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -599,15 +603,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="W5" sqref="W5"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="38" customWidth="1"/>
+    <col min="13" max="13" width="27.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -703,7 +711,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3516</v>
       </c>
@@ -786,7 +794,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3517</v>
       </c>
@@ -869,7 +877,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3518</v>
       </c>
@@ -952,7 +960,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3519</v>
       </c>
@@ -1035,7 +1043,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3520</v>
       </c>
@@ -1118,7 +1126,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>16390</v>
       </c>
@@ -1201,7 +1209,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>16391</v>
       </c>
@@ -1284,7 +1292,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>21575</v>
       </c>
@@ -1367,7 +1375,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>45978</v>
       </c>
@@ -1450,7 +1458,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>62693</v>
       </c>
@@ -1533,7 +1541,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>62694</v>
       </c>
@@ -1616,7 +1624,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>62695</v>
       </c>
@@ -1699,7 +1707,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>62696</v>
       </c>
@@ -1782,7 +1790,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>62697</v>
       </c>
@@ -1865,7 +1873,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>62698</v>
       </c>
@@ -1948,7 +1956,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>62699</v>
       </c>
@@ -2031,7 +2039,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>62700</v>
       </c>
@@ -2114,7 +2122,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>62701</v>
       </c>
@@ -2197,7 +2205,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>62702</v>
       </c>
@@ -2280,7 +2288,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>62703</v>
       </c>
@@ -2363,7 +2371,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>62704</v>
       </c>
@@ -2446,7 +2454,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>62705</v>
       </c>
@@ -2529,7 +2537,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>212837</v>
       </c>

</xml_diff>

<commit_message>
feat: implement LLM-powered PO query system with conversation memory and database migration
</commit_message>
<xml_diff>
--- a/06.adhoc.requests/18.substations/Subcontractor_Details_substations_equipment.xlsx
+++ b/06.adhoc.requests/18.substations/Subcontractor_Details_substations_equipment.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://rowadmodern-my.sharepoint.com/personal/omar_essam_rowad-rme_com/Documents/x004 Data Science/03.rme.db/00.repo/rme.db/06.adhoc.requests/18.substations/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{1257172F-23D5-4CA5-87EE-B0EF93EC9159}"/>
+  <xr:revisionPtr revIDLastSave="7" documentId="11_F25DC773A252ABDACC1048BDC11F63425BDE58E3" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{B7174F25-C307-442D-9DE0-8D418B4A020A}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -332,6 +332,10 @@
     </ext>
   </extLst>
 </styleSheet>
+</file>
+
+<file path=xl/persons/person.xml><?xml version="1.0" encoding="utf-8"?>
+<personList xmlns="http://schemas.microsoft.com/office/spreadsheetml/2018/threadedcomments" xmlns:x="http://schemas.openxmlformats.org/spreadsheetml/2006/main"/>
 </file>
 
 <file path=xl/theme/theme1.xml><?xml version="1.0" encoding="utf-8"?>
@@ -599,15 +603,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:AF24"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="K1" workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <pane ySplit="1" topLeftCell="A2" activePane="bottomLeft" state="frozen"/>
       <selection activeCell="K1" sqref="K1"/>
-      <selection pane="bottomLeft" activeCell="W5" sqref="W5"/>
+      <selection pane="bottomLeft" activeCell="L11" sqref="L11"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
+  <cols>
+    <col min="5" max="5" width="38" customWidth="1"/>
+    <col min="13" max="13" width="27.44140625" customWidth="1"/>
+  </cols>
   <sheetData>
-    <row r="1" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A1" s="1"/>
       <c r="B1" s="1" t="s">
         <v>0</v>
@@ -703,7 +711,7 @@
         <v>27</v>
       </c>
     </row>
-    <row r="2" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A2">
         <v>3516</v>
       </c>
@@ -786,7 +794,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="3" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A3">
         <v>3517</v>
       </c>
@@ -869,7 +877,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="4" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A4">
         <v>3518</v>
       </c>
@@ -952,7 +960,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="5" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A5">
         <v>3519</v>
       </c>
@@ -1035,7 +1043,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="6" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A6">
         <v>3520</v>
       </c>
@@ -1118,7 +1126,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="7" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A7">
         <v>16390</v>
       </c>
@@ -1201,7 +1209,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="8" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A8">
         <v>16391</v>
       </c>
@@ -1284,7 +1292,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="9" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A9">
         <v>21575</v>
       </c>
@@ -1367,7 +1375,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="10" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A10">
         <v>45978</v>
       </c>
@@ -1450,7 +1458,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="11" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A11">
         <v>62693</v>
       </c>
@@ -1533,7 +1541,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="12" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A12">
         <v>62694</v>
       </c>
@@ -1616,7 +1624,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="13" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A13">
         <v>62695</v>
       </c>
@@ -1699,7 +1707,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="14" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A14">
         <v>62696</v>
       </c>
@@ -1782,7 +1790,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="15" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A15">
         <v>62697</v>
       </c>
@@ -1865,7 +1873,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="16" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A16">
         <v>62698</v>
       </c>
@@ -1948,7 +1956,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="17" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A17">
         <v>62699</v>
       </c>
@@ -2031,7 +2039,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="18" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A18">
         <v>62700</v>
       </c>
@@ -2114,7 +2122,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="19" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A19">
         <v>62701</v>
       </c>
@@ -2197,7 +2205,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="20" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A20">
         <v>62702</v>
       </c>
@@ -2280,7 +2288,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="21" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A21">
         <v>62703</v>
       </c>
@@ -2363,7 +2371,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="22" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A22">
         <v>62704</v>
       </c>
@@ -2446,7 +2454,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="23" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A23">
         <v>62705</v>
       </c>
@@ -2529,7 +2537,7 @@
         <v>41</v>
       </c>
     </row>
-    <row r="24" spans="1:32" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:32" x14ac:dyDescent="0.3">
       <c r="A24">
         <v>212837</v>
       </c>

</xml_diff>